<commit_message>
Stu updates to list
</commit_message>
<xml_diff>
--- a/misc_notes/Tasks for LitScan tool 6 Jul 2023.xlsx
+++ b/misc_notes/Tasks for LitScan tool 6 Jul 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\12 Research\Oxbury et al Automating literature searches for RL assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C378AA9-05F1-45FE-A349-46E0B3DB3050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB6BFC5-2999-41AD-AAE8-8ED0370D1C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9EB13B81-855B-4288-A8E6-06B24F85ECDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9EB13B81-855B-4288-A8E6-06B24F85ECDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>Complete migration to Azure VM</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Agree BirdLife adoption route (LitScan is currently hosted in an isolated Azure subscription, which prevents BirdLife access to LitScan file shares) So a plan is needed on the expected resourcing for operational management of the tool. This in turn will affect requirements for the Azure architecture.</t>
   </si>
   <si>
-    <t>Add new sources in response to user requests (e.g. specific searching of Notornis, Ostritch and Kukila journal websites, and the abstract database Scopus. Possibly ResearchGate?)</t>
-  </si>
-  <si>
     <t>OpenAlex scan needs fixing in response to undiagnosed API changes</t>
   </si>
   <si>
@@ -126,6 +123,21 @@
   </si>
   <si>
     <t>Fix PDF upload at the firewall (currently works up to AG) (i.e. functionality to allow assessors to upload pdfs of relevant reports and OBC/ABC/NBC journals and pre-assign relevance scores)</t>
+  </si>
+  <si>
+    <t>Add new sources in response to user requests (e.g. specific searching of Notornis, Ostritch and Kukila journal websites, and the abstract database Scopus. Possibly ResearchGate?). Enable Bing search through discussion with MicroSoft again.</t>
+  </si>
+  <si>
+    <t>Must/Should/Could/Will not have for MVP</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>S/C</t>
+  </si>
+  <si>
+    <t>W but good to think through the possibilities here soon</t>
   </si>
 </sst>
 </file>
@@ -493,29 +505,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C44B63A-7A1A-4134-AA34-1E391E02A6AC}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19:XFD19"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="98.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -523,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -531,7 +547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -539,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -547,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -555,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -563,7 +579,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -571,7 +587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -579,15 +595,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -595,7 +614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -603,31 +622,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -635,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -643,7 +668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -651,15 +676,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -667,7 +695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -675,15 +703,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -691,7 +722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -699,7 +730,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>

</xml_diff>